<commit_message>
Chỉnh sửa, bắt lỗi
</commit_message>
<xml_diff>
--- a/Project_DataWarehouse/files/sinhvien/sinhvien_chieu_nhom12.xls.xlsx
+++ b/Project_DataWarehouse/files/sinhvien/sinhvien_chieu_nhom12.xls.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuong Tu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevPrograms\git\DataWarehouse_nhom14\Project_DataWarehouse\files\sinhvien\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F232C66-CFC6-41C6-A3F5-ED126DA4430E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2426,7 +2427,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2923,11 +2924,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B151" workbookViewId="0">
-      <selection activeCell="J222" sqref="J222"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9911,8 +9912,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3:I217" r:id="rId2" display="dovanc@gmail.com.vn"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I3:I217" r:id="rId2" display="dovanc@gmail.com.vn" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>